<commit_message>
v1.8.1 add data 2021 08 09
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/pinyin/20210604.xlsx
+++ b/ai/assets/textbook/pinyin/20210604.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessie.chiao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\pinyin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E1D1C2-8FC7-4169-B5AB-1C2D466EC7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="15915" windowHeight="15600"/>
+    <workbookView xWindow="-18765" yWindow="465" windowWidth="17880" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1946,8 +1947,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2309,20 +2310,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="71.75" customWidth="1"/>
     <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33">
+    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -2346,7 +2347,7 @@
       <c r="C2" s="2"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2356,7 +2357,7 @@
       <c r="C3" s="2"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2366,7 +2367,7 @@
       <c r="C4" s="2"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2377,7 @@
       <c r="C5" s="2"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -2386,7 +2387,7 @@
       <c r="C6" s="2"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2396,7 +2397,7 @@
       <c r="C7" s="2"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2406,7 +2407,7 @@
       <c r="C8" s="2"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -2416,7 +2417,7 @@
       <c r="C9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1">
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>151</v>
       </c>
@@ -2426,7 +2427,7 @@
       <c r="C10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -2436,7 +2437,7 @@
       <c r="C11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>160</v>
       </c>
@@ -2446,7 +2447,7 @@
       <c r="C12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>185</v>
       </c>
@@ -2456,7 +2457,7 @@
       <c r="C13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>186</v>
       </c>
@@ -2466,7 +2467,7 @@
       <c r="C14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>187</v>
       </c>
@@ -2476,7 +2477,7 @@
       <c r="C15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>188</v>
       </c>
@@ -2486,7 +2487,7 @@
       <c r="C16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>198</v>
       </c>
@@ -2496,7 +2497,7 @@
       <c r="C17" s="2"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>545</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>547</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2546,7 +2547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2659,7 +2660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
@@ -2789,7 +2790,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>55</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>59</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -2915,7 +2916,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -2929,7 +2930,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>64</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>66</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>67</v>
       </c>
@@ -2982,7 +2983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
@@ -2993,7 +2994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>69</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -3046,7 +3047,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
@@ -3071,7 +3072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
@@ -3085,7 +3086,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>79</v>
       </c>
@@ -3099,7 +3100,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>81</v>
       </c>
@@ -3113,7 +3114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>82</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>83</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>84</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>85</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>87</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>88</v>
       </c>
@@ -3197,7 +3198,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>89</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>91</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>92</v>
       </c>
@@ -3239,7 +3240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>93</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>95</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>98</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>100</v>
       </c>
@@ -3306,7 +3307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>110</v>
       </c>
@@ -3320,7 +3321,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>102</v>
       </c>
@@ -3334,7 +3335,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>103</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>104</v>
       </c>
@@ -3362,7 +3363,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>105</v>
       </c>
@@ -3376,7 +3377,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>106</v>
       </c>
@@ -3390,7 +3391,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>107</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>108</v>
       </c>
@@ -3418,7 +3419,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>109</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>114</v>
       </c>
@@ -3446,7 +3447,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>116</v>
       </c>
@@ -3460,7 +3461,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>118</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>119</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>121</v>
       </c>
@@ -3499,7 +3500,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>123</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>124</v>
       </c>
@@ -3527,7 +3528,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>126</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>128</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>129</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>130</v>
       </c>
@@ -3583,7 +3584,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>131</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>133</v>
       </c>
@@ -3611,7 +3612,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>134</v>
       </c>
@@ -3625,7 +3626,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>135</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>137</v>
       </c>
@@ -3653,7 +3654,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>139</v>
       </c>
@@ -3667,7 +3668,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>140</v>
       </c>
@@ -3681,7 +3682,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>141</v>
       </c>
@@ -3695,7 +3696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>142</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>144</v>
       </c>
@@ -3723,7 +3724,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>145</v>
       </c>
@@ -3737,7 +3738,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>146</v>
       </c>
@@ -3751,7 +3752,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>148</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>149</v>
       </c>
@@ -3779,7 +3780,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>150</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>153</v>
       </c>
@@ -3804,7 +3805,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>155</v>
       </c>
@@ -3818,7 +3819,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>157</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>159</v>
       </c>
@@ -3846,7 +3847,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>161</v>
       </c>
@@ -3860,7 +3861,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>163</v>
       </c>
@@ -3874,7 +3875,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>165</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>166</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>169</v>
       </c>
@@ -3916,7 +3917,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>171</v>
       </c>
@@ -3930,7 +3931,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>172</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>174</v>
       </c>
@@ -3958,7 +3959,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>176</v>
       </c>
@@ -3972,7 +3973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>177</v>
       </c>
@@ -3986,7 +3987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>178</v>
       </c>
@@ -4000,7 +4001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>179</v>
       </c>
@@ -4014,7 +4015,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>181</v>
       </c>
@@ -4028,7 +4029,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>182</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>183</v>
       </c>
@@ -4056,7 +4057,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>184</v>
       </c>
@@ -4070,7 +4071,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>190</v>
       </c>
@@ -4084,7 +4085,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>189</v>
       </c>
@@ -4098,7 +4099,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>192</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>194</v>
       </c>
@@ -4123,7 +4124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>195</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>197</v>
       </c>
@@ -4148,7 +4149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>199</v>
       </c>
@@ -4159,7 +4160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>200</v>
       </c>
@@ -4173,7 +4174,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>202</v>
       </c>
@@ -4187,7 +4188,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>204</v>
       </c>
@@ -4201,7 +4202,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>206</v>
       </c>
@@ -4212,7 +4213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>210</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>207</v>
       </c>
@@ -4240,7 +4241,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>208</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>209</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>212</v>
       </c>
@@ -4279,7 +4280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>213</v>
       </c>
@@ -4290,7 +4291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>214</v>
       </c>
@@ -4304,7 +4305,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>215</v>
       </c>
@@ -4318,7 +4319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>216</v>
       </c>
@@ -4332,7 +4333,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>218</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>220</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>221</v>
       </c>
@@ -4374,7 +4375,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>222</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>224</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>226</v>
       </c>
@@ -4416,7 +4417,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>228</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>230</v>
       </c>
@@ -4441,7 +4442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>231</v>
       </c>
@@ -4452,7 +4453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>232</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>233</v>
       </c>
@@ -4477,7 +4478,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>235</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>237</v>
       </c>
@@ -4505,7 +4506,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>240</v>
       </c>
@@ -4519,7 +4520,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>241</v>
       </c>
@@ -4533,7 +4534,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>243</v>
       </c>
@@ -4547,7 +4548,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>246</v>
       </c>
@@ -4561,7 +4562,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>247</v>
       </c>
@@ -4575,7 +4576,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>248</v>
       </c>
@@ -4589,7 +4590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>250</v>
       </c>
@@ -4603,7 +4604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>251</v>
       </c>
@@ -4617,7 +4618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>252</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>254</v>
       </c>
@@ -4645,7 +4646,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>257</v>
       </c>
@@ -4659,7 +4660,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>259</v>
       </c>
@@ -4673,7 +4674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>260</v>
       </c>
@@ -4687,7 +4688,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>262</v>
       </c>
@@ -4701,7 +4702,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>264</v>
       </c>
@@ -4715,7 +4716,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>266</v>
       </c>
@@ -4729,7 +4730,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>267</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>269</v>
       </c>
@@ -4757,7 +4758,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>271</v>
       </c>
@@ -4771,7 +4772,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>273</v>
       </c>
@@ -4782,7 +4783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>274</v>
       </c>
@@ -4793,7 +4794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>275</v>
       </c>
@@ -4804,7 +4805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>276</v>
       </c>
@@ -4815,7 +4816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>277</v>
       </c>
@@ -4826,7 +4827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>278</v>
       </c>
@@ -4840,7 +4841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>279</v>
       </c>
@@ -4854,7 +4855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>280</v>
       </c>
@@ -4868,7 +4869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>281</v>
       </c>
@@ -4882,7 +4883,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>283</v>
       </c>
@@ -4896,7 +4897,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>285</v>
       </c>
@@ -4910,7 +4911,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>286</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>288</v>
       </c>
@@ -4938,7 +4939,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>289</v>
       </c>
@@ -4952,7 +4953,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>290</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>293</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>295</v>
       </c>
@@ -4991,7 +4992,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>291</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>292</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>297</v>
       </c>
@@ -5033,7 +5034,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>299</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>302</v>
       </c>
@@ -5061,7 +5062,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>303</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>305</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>306</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>308</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>309</v>
       </c>
@@ -5131,7 +5132,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>310</v>
       </c>
@@ -5145,7 +5146,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>312</v>
       </c>
@@ -5156,7 +5157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>313</v>
       </c>
@@ -5167,7 +5168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>314</v>
       </c>
@@ -5181,7 +5182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>315</v>
       </c>
@@ -5195,7 +5196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>316</v>
       </c>
@@ -5209,7 +5210,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>317</v>
       </c>
@@ -5223,7 +5224,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>318</v>
       </c>
@@ -5237,7 +5238,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>320</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>322</v>
       </c>
@@ -5265,7 +5266,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>323</v>
       </c>
@@ -5279,7 +5280,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>324</v>
       </c>
@@ -5293,7 +5294,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>325</v>
       </c>
@@ -5307,7 +5308,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>326</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>327</v>
       </c>
@@ -5335,7 +5336,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>328</v>
       </c>
@@ -5349,7 +5350,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>329</v>
       </c>
@@ -5363,7 +5364,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>330</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>331</v>
       </c>
@@ -5391,7 +5392,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>332</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>334</v>
       </c>
@@ -5419,7 +5420,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>336</v>
       </c>
@@ -5433,7 +5434,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>338</v>
       </c>
@@ -5447,7 +5448,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>340</v>
       </c>
@@ -5461,7 +5462,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>341</v>
       </c>
@@ -5475,7 +5476,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>342</v>
       </c>
@@ -5489,7 +5490,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>344</v>
       </c>
@@ -5503,7 +5504,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>345</v>
       </c>
@@ -5517,7 +5518,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>346</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>347</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>348</v>
       </c>
@@ -5559,7 +5560,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>349</v>
       </c>
@@ -5573,7 +5574,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>350</v>
       </c>
@@ -5587,7 +5588,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="248" spans="1:5">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>351</v>
       </c>
@@ -5601,7 +5602,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>352</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>355</v>
       </c>
@@ -5629,7 +5630,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>356</v>
       </c>
@@ -5643,7 +5644,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>357</v>
       </c>
@@ -5657,7 +5658,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>359</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>361</v>
       </c>
@@ -5685,7 +5686,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="255" spans="1:5">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>362</v>
       </c>
@@ -5699,7 +5700,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>363</v>
       </c>
@@ -5713,7 +5714,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="257" spans="1:5">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>364</v>
       </c>
@@ -5727,7 +5728,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="258" spans="1:5">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>365</v>
       </c>
@@ -5741,7 +5742,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>366</v>
       </c>
@@ -5755,7 +5756,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="260" spans="1:5">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>368</v>
       </c>
@@ -5769,7 +5770,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>369</v>
       </c>
@@ -5783,7 +5784,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>370</v>
       </c>
@@ -5797,7 +5798,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>371</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>372</v>
       </c>
@@ -5825,7 +5826,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>373</v>
       </c>
@@ -5839,7 +5840,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>374</v>
       </c>
@@ -5853,7 +5854,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>375</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>377</v>
       </c>
@@ -5881,7 +5882,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>379</v>
       </c>
@@ -5895,7 +5896,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>381</v>
       </c>
@@ -5909,7 +5910,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="271" spans="1:5">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>382</v>
       </c>
@@ -5923,7 +5924,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="272" spans="1:5">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>383</v>
       </c>
@@ -5937,7 +5938,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>385</v>
       </c>
@@ -5951,7 +5952,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>386</v>
       </c>
@@ -5965,7 +5966,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="275" spans="1:5">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>388</v>
       </c>
@@ -5979,7 +5980,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="276" spans="1:5">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>390</v>
       </c>
@@ -5993,7 +5994,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="277" spans="1:5">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>392</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="278" spans="1:5">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>393</v>
       </c>
@@ -6021,7 +6022,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>394</v>
       </c>
@@ -6035,7 +6036,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>395</v>
       </c>
@@ -6049,7 +6050,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>396</v>
       </c>
@@ -6063,7 +6064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>397</v>
       </c>
@@ -6077,7 +6078,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>399</v>
       </c>
@@ -6091,7 +6092,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>400</v>
       </c>
@@ -6105,7 +6106,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>401</v>
       </c>
@@ -6119,7 +6120,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="286" spans="1:5">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>402</v>
       </c>
@@ -6133,7 +6134,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="287" spans="1:5">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>403</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>404</v>
       </c>
@@ -6161,7 +6162,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>406</v>
       </c>
@@ -6175,7 +6176,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="290" spans="1:5">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>407</v>
       </c>
@@ -6189,7 +6190,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="291" spans="1:5">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>408</v>
       </c>
@@ -6203,7 +6204,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="292" spans="1:5">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>409</v>
       </c>
@@ -6217,7 +6218,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="293" spans="1:5">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>410</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="294" spans="1:5">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>411</v>
       </c>
@@ -6245,7 +6246,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="295" spans="1:5">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>412</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="296" spans="1:5">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>414</v>
       </c>
@@ -6273,7 +6274,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="297" spans="1:5">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>416</v>
       </c>
@@ -6287,7 +6288,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="298" spans="1:5">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>417</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>419</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="300" spans="1:5">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>420</v>
       </c>
@@ -6329,7 +6330,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="301" spans="1:5">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>421</v>
       </c>
@@ -6343,7 +6344,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="302" spans="1:5">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>422</v>
       </c>
@@ -6354,7 +6355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:5">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>423</v>
       </c>
@@ -6365,7 +6366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:5">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>424</v>
       </c>
@@ -6376,7 +6377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>425</v>
       </c>
@@ -6390,7 +6391,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="306" spans="1:5">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>427</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:5">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>428</v>
       </c>
@@ -6415,7 +6416,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>430</v>
       </c>
@@ -6429,7 +6430,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="309" spans="1:5">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>432</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="310" spans="1:5">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>433</v>
       </c>
@@ -6457,7 +6458,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="311" spans="1:5">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>434</v>
       </c>
@@ -6471,7 +6472,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="312" spans="1:5">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>436</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="313" spans="1:5">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>438</v>
       </c>
@@ -6499,7 +6500,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="314" spans="1:5">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>440</v>
       </c>
@@ -6513,7 +6514,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="315" spans="1:5">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>442</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="316" spans="1:5">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>443</v>
       </c>
@@ -6541,7 +6542,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="317" spans="1:5">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>444</v>
       </c>
@@ -6552,7 +6553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="318" spans="1:5">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>445</v>
       </c>
@@ -6563,7 +6564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="319" spans="1:5">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>446</v>
       </c>
@@ -6574,7 +6575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="1:5">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>447</v>
       </c>
@@ -6585,7 +6586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>448</v>
       </c>
@@ -6596,7 +6597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>449</v>
       </c>
@@ -6607,7 +6608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>450</v>
       </c>
@@ -6618,7 +6619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>451</v>
       </c>
@@ -6629,7 +6630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>452</v>
       </c>
@@ -6640,7 +6641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>453</v>
       </c>
@@ -6651,7 +6652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>454</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>455</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>456</v>
       </c>
@@ -6684,7 +6685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>457</v>
       </c>
@@ -6695,7 +6696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>458</v>
       </c>
@@ -6706,7 +6707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>459</v>
       </c>
@@ -6717,7 +6718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>460</v>
       </c>
@@ -6728,7 +6729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>461</v>
       </c>
@@ -6739,7 +6740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>462</v>
       </c>
@@ -6750,7 +6751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>463</v>
       </c>
@@ -6761,7 +6762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>464</v>
       </c>
@@ -6772,7 +6773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>465</v>
       </c>
@@ -6783,7 +6784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>466</v>
       </c>
@@ -6794,7 +6795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="340" spans="1:3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>467</v>
       </c>
@@ -6805,7 +6806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>468</v>
       </c>
@@ -6816,7 +6817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>469</v>
       </c>
@@ -6827,7 +6828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:3">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>470</v>
       </c>
@@ -6838,7 +6839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>471</v>
       </c>
@@ -6849,7 +6850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>472</v>
       </c>
@@ -6860,7 +6861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>473</v>
       </c>
@@ -6871,7 +6872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>474</v>
       </c>
@@ -6882,7 +6883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>475</v>
       </c>
@@ -6893,7 +6894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="349" spans="1:3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>476</v>
       </c>
@@ -6904,7 +6905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="350" spans="1:3">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>477</v>
       </c>
@@ -6915,7 +6916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="351" spans="1:3">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>478</v>
       </c>
@@ -6926,7 +6927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="352" spans="1:3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>479</v>
       </c>
@@ -6937,7 +6938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="353" spans="1:3">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>480</v>
       </c>
@@ -6948,7 +6949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>481</v>
       </c>
@@ -6959,7 +6960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="355" spans="1:3">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>482</v>
       </c>
@@ -6970,7 +6971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="356" spans="1:3">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>483</v>
       </c>
@@ -6981,7 +6982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="357" spans="1:3">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>484</v>
       </c>
@@ -6992,7 +6993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:3">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>485</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="359" spans="1:3">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>486</v>
       </c>
@@ -7014,7 +7015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="360" spans="1:3">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>15</v>
       </c>
@@ -7025,7 +7026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="361" spans="1:3">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>487</v>
       </c>
@@ -7036,7 +7037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="362" spans="1:3">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>488</v>
       </c>
@@ -7047,7 +7048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="363" spans="1:3">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>16</v>
       </c>
@@ -7058,7 +7059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="364" spans="1:3">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>489</v>
       </c>
@@ -7069,7 +7070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="365" spans="1:3">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>490</v>
       </c>
@@ -7080,7 +7081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="366" spans="1:3">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>491</v>
       </c>
@@ -7091,7 +7092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="367" spans="1:3">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>492</v>
       </c>
@@ -7102,7 +7103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="368" spans="1:3">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>493</v>
       </c>
@@ -7113,7 +7114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="369" spans="1:3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>494</v>
       </c>
@@ -7124,7 +7125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>496</v>
       </c>
@@ -7135,7 +7136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="371" spans="1:3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>495</v>
       </c>
@@ -7146,7 +7147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="372" spans="1:3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>497</v>
       </c>
@@ -7157,7 +7158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="373" spans="1:3">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>498</v>
       </c>
@@ -7168,7 +7169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:3">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>499</v>
       </c>
@@ -7179,7 +7180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="375" spans="1:3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>500</v>
       </c>
@@ -7190,7 +7191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:3">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>501</v>
       </c>
@@ -7201,7 +7202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>502</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>503</v>
       </c>
@@ -7223,7 +7224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="379" spans="1:3">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>504</v>
       </c>
@@ -7234,7 +7235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="380" spans="1:3">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>505</v>
       </c>
@@ -7245,7 +7246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="381" spans="1:3">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>506</v>
       </c>
@@ -7256,7 +7257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>507</v>
       </c>
@@ -7267,7 +7268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="383" spans="1:3">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>508</v>
       </c>
@@ -7278,7 +7279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="384" spans="1:3">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>509</v>
       </c>
@@ -7289,7 +7290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="385" spans="1:3">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>510</v>
       </c>
@@ -7300,7 +7301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="386" spans="1:3">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>511</v>
       </c>
@@ -7311,7 +7312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="387" spans="1:3">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>512</v>
       </c>
@@ -7322,7 +7323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="388" spans="1:3">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>513</v>
       </c>
@@ -7333,7 +7334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="389" spans="1:3">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>514</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="390" spans="1:3">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>515</v>
       </c>
@@ -7355,7 +7356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="391" spans="1:3">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>516</v>
       </c>
@@ -7366,7 +7367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="392" spans="1:3">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>517</v>
       </c>
@@ -7377,7 +7378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="1:3">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>518</v>
       </c>
@@ -7388,7 +7389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="394" spans="1:3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>519</v>
       </c>
@@ -7399,7 +7400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="395" spans="1:3">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>520</v>
       </c>
@@ -7410,7 +7411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="396" spans="1:3">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>521</v>
       </c>
@@ -7421,7 +7422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="397" spans="1:3">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>522</v>
       </c>
@@ -7432,7 +7433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="398" spans="1:3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>523</v>
       </c>
@@ -7443,7 +7444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="399" spans="1:3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>524</v>
       </c>
@@ -7454,7 +7455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="400" spans="1:3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>525</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="1:3">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>526</v>
       </c>
@@ -7476,7 +7477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="1:3">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>527</v>
       </c>
@@ -7487,7 +7488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="403" spans="1:3">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>528</v>
       </c>
@@ -7498,7 +7499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="404" spans="1:3">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>529</v>
       </c>
@@ -7509,7 +7510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="405" spans="1:3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>530</v>
       </c>
@@ -7520,7 +7521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="406" spans="1:3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>531</v>
       </c>
@@ -7531,7 +7532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="407" spans="1:3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>532</v>
       </c>
@@ -7542,7 +7543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="408" spans="1:3">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>533</v>
       </c>
@@ -7553,7 +7554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="409" spans="1:3">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>534</v>
       </c>
@@ -7564,7 +7565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="410" spans="1:3">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>535</v>
       </c>
@@ -7575,7 +7576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="411" spans="1:3">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>536</v>
       </c>
@@ -7586,7 +7587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="412" spans="1:3">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>537</v>
       </c>
@@ -7597,7 +7598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="413" spans="1:3">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>538</v>
       </c>
@@ -7608,7 +7609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="414" spans="1:3">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>539</v>
       </c>
@@ -7619,7 +7620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="415" spans="1:3">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>540</v>
       </c>
@@ -7630,7 +7631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="416" spans="1:3">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>541</v>
       </c>
@@ -7641,7 +7642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="417" spans="1:3">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>542</v>
       </c>
@@ -7652,7 +7653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="418" spans="1:3">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>543</v>
       </c>
@@ -7663,7 +7664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="419" spans="1:3">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>544</v>
       </c>
@@ -7674,148 +7675,148 @@
         <v>3</v>
       </c>
     </row>
-    <row r="420" spans="1:3">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1"/>
     </row>
-    <row r="421" spans="1:3">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1"/>
     </row>
-    <row r="422" spans="1:3">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1"/>
     </row>
-    <row r="423" spans="1:3">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1"/>
     </row>
-    <row r="424" spans="1:3">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1"/>
     </row>
-    <row r="425" spans="1:3">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1"/>
     </row>
-    <row r="426" spans="1:3">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1"/>
     </row>
-    <row r="427" spans="1:3">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1"/>
     </row>
-    <row r="428" spans="1:3">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1"/>
     </row>
-    <row r="429" spans="1:3">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1"/>
     </row>
-    <row r="430" spans="1:3">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1"/>
     </row>
-    <row r="431" spans="1:3">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1"/>
     </row>
-    <row r="432" spans="1:3">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1"/>
     </row>
-    <row r="433" spans="1:1">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="1"/>
     </row>
-    <row r="434" spans="1:1">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="1"/>
     </row>
-    <row r="435" spans="1:1">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" s="1"/>
     </row>
-    <row r="436" spans="1:1">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="1"/>
     </row>
-    <row r="437" spans="1:1">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="1"/>
     </row>
-    <row r="438" spans="1:1">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" s="1"/>
     </row>
-    <row r="439" spans="1:1">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="1"/>
     </row>
-    <row r="440" spans="1:1">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" s="1"/>
     </row>
-    <row r="441" spans="1:1">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" s="1"/>
     </row>
-    <row r="442" spans="1:1">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="1"/>
     </row>
-    <row r="443" spans="1:1">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="1"/>
     </row>
-    <row r="444" spans="1:1">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" s="1"/>
     </row>
-    <row r="445" spans="1:1">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="1"/>
     </row>
-    <row r="446" spans="1:1">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="1"/>
     </row>
-    <row r="447" spans="1:1">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="1"/>
     </row>
-    <row r="448" spans="1:1">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" s="1"/>
     </row>
-    <row r="449" spans="1:1">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="1"/>
     </row>
-    <row r="450" spans="1:1">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" s="1"/>
     </row>
-    <row r="451" spans="1:1">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" s="1"/>
     </row>
-    <row r="452" spans="1:1">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" s="1"/>
     </row>
-    <row r="453" spans="1:1">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" s="1"/>
     </row>
-    <row r="454" spans="1:1">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" s="1"/>
     </row>
-    <row r="455" spans="1:1">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="1"/>
     </row>
-    <row r="456" spans="1:1">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" s="1"/>
     </row>
-    <row r="457" spans="1:1">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" s="1"/>
     </row>
-    <row r="458" spans="1:1">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" s="1"/>
     </row>
-    <row r="459" spans="1:1">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" s="1"/>
     </row>
-    <row r="460" spans="1:1">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" s="1"/>
     </row>
-    <row r="461" spans="1:1">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="1"/>
     </row>
-    <row r="462" spans="1:1">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" s="1"/>
     </row>
-    <row r="463" spans="1:1">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" s="1"/>
     </row>
-    <row r="464" spans="1:1">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" s="1"/>
     </row>
-    <row r="465" spans="1:1">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" s="1"/>
     </row>
-    <row r="466" spans="1:1">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" s="1"/>
     </row>
-    <row r="467" spans="1:1">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" s="1"/>
     </row>
   </sheetData>

</xml_diff>